<commit_message>
Give preference to courses with more students and assign values well
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MAT141</t>
+          <t>SOC205</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -481,7 +481,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -498,7 +498,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SOC205</t>
+          <t>MAT141</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -508,7 +508,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -539,11 +539,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>KDLT</t>
+          <t>SLT</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -566,11 +566,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>FLT</t>
+          <t>KDLT</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
@@ -593,11 +593,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>NFLT</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>50</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7">
@@ -620,11 +620,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>FLT</t>
+          <t>CBN</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
     <row r="8">
@@ -647,11 +647,13 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>KDLT</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>150</v>
+          <t>No suitable venue</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -701,11 +703,11 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>KDLT</t>
+          <t>SLT</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -741,7 +743,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BIO101</t>
+          <t>PSY101</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -751,15 +753,15 @@
         <v>16</v>
       </c>
       <c r="E12" t="n">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>FLT</t>
+          <t>KDLT</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13">
@@ -768,7 +770,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PSY101</t>
+          <t>BIO101</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -778,15 +780,15 @@
         <v>16</v>
       </c>
       <c r="E13" t="n">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>KDLT</t>
+          <t>NFLT</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>150</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14">
@@ -836,11 +838,11 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>KDLT</t>
+          <t>CBN</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>150</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
Make times datetime object instead of integers
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -471,17 +471,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SOC205</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>8</v>
-      </c>
-      <c r="D2" t="n">
-        <v>11</v>
+          <t>MAT141</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
       </c>
       <c r="E2" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -498,17 +502,21 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MAT141</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>8</v>
-      </c>
-      <c r="D3" t="n">
-        <v>11</v>
+          <t>SOC205</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>08:30</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
       </c>
       <c r="E3" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -528,11 +536,15 @@
           <t>PHY201</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D4" t="n">
-        <v>12</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
       </c>
       <c r="E4" t="n">
         <v>70</v>
@@ -555,11 +567,15 @@
           <t>ECON202</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>9</v>
-      </c>
-      <c r="D5" t="n">
-        <v>12</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>09:30</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
       </c>
       <c r="E5" t="n">
         <v>55</v>
@@ -582,11 +598,15 @@
           <t>CSC103</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" t="n">
-        <v>13</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
       </c>
       <c r="E6" t="n">
         <v>50</v>
@@ -609,11 +629,15 @@
           <t>ENG220</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>10</v>
-      </c>
-      <c r="D7" t="n">
-        <v>13</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
       </c>
       <c r="E7" t="n">
         <v>25</v>
@@ -636,11 +660,15 @@
           <t>STA121</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>11</v>
-      </c>
-      <c r="D8" t="n">
-        <v>14</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
       </c>
       <c r="E8" t="n">
         <v>140</v>
@@ -650,10 +678,8 @@
           <t>No suitable venue</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
+      <c r="G8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -665,11 +691,15 @@
           <t>GEO111</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>11</v>
-      </c>
-      <c r="D9" t="n">
-        <v>14</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
       </c>
       <c r="E9" t="n">
         <v>75</v>
@@ -692,11 +722,15 @@
           <t>HIS101</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>12</v>
-      </c>
-      <c r="D10" t="n">
-        <v>15</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
       </c>
       <c r="E10" t="n">
         <v>80</v>
@@ -719,11 +753,15 @@
           <t>MUS120</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>12</v>
-      </c>
-      <c r="D11" t="n">
-        <v>15</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>15:30</t>
+        </is>
       </c>
       <c r="E11" t="n">
         <v>20</v>
@@ -743,17 +781,21 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>PSY101</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>13</v>
-      </c>
-      <c r="D12" t="n">
-        <v>16</v>
+          <t>BIO101</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
       </c>
       <c r="E12" t="n">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -770,17 +812,21 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BIO101</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>13</v>
-      </c>
-      <c r="D13" t="n">
-        <v>16</v>
+          <t>PSY101</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
       </c>
       <c r="E13" t="n">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -800,22 +846,26 @@
           <t>CSC103</t>
         </is>
       </c>
-      <c r="C14" t="n">
-        <v>14</v>
-      </c>
-      <c r="D14" t="n">
-        <v>17</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
       </c>
       <c r="E14" t="n">
         <v>90</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>FLT</t>
+          <t>CBN</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15">
@@ -827,22 +877,26 @@
           <t>CHEM301</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>14</v>
-      </c>
-      <c r="D15" t="n">
-        <v>17</v>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
       </c>
       <c r="E15" t="n">
         <v>60</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>CBN</t>
+          <t>FLT</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16">
@@ -854,22 +908,26 @@
           <t>ART150</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>15</v>
-      </c>
-      <c r="D16" t="n">
-        <v>18</v>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
       </c>
       <c r="E16" t="n">
         <v>35</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>SLT</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>